<commit_message>
Update {t,b}values locations; add R17 to BOM
</commit_message>
<xml_diff>
--- a/hardware/impulse/rev_c/impulse_bom.xlsx
+++ b/hardware/impulse/rev_c/impulse_bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="119">
   <si>
     <t>Qty</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>RHM5.1MBICT-ND</t>
+  </si>
+  <si>
+    <t>0k</t>
+  </si>
+  <si>
+    <t>R17</t>
   </si>
   <si>
     <t>DS2411</t>
@@ -492,10 +498,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F12" activeCellId="0" pane="topLeft" sqref="F12"/>
+      <selection activeCell="G25" activeCellId="0" pane="topLeft" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1056,45 +1062,40 @@
         <v>89</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D25" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>91</v>
-      </c>
       <c r="F25" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>93</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G25" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="0" t="s">
+      <c r="G26" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
@@ -1102,62 +1103,68 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="0" t="s">
+      <c r="H27" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="C28" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
-      <c r="A28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="E28" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="0" t="s">
+      <c r="G28" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="29">
+      <c r="A29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="C29" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="E29" s="0" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
-      <c r="A29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="F29" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="0" t="s">
+      <c r="G29" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
@@ -1165,22 +1172,42 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="0" t="s">
+      <c r="G30" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E30" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="A31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="C31" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="E31" s="0" t="s">
         <v>116</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated doc for impulse rev c
</commit_message>
<xml_diff>
--- a/hardware/impulse/rev_c/impulse_bom.xlsx
+++ b/hardware/impulse/rev_c/impulse_bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>Qty</t>
   </si>
@@ -282,12 +282,6 @@
   </si>
   <si>
     <t>RHM5.1MBICT-ND</t>
-  </si>
-  <si>
-    <t>0k</t>
-  </si>
-  <si>
-    <t>R17</t>
   </si>
   <si>
     <t>DS2411</t>
@@ -498,10 +492,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G25" activeCellId="0" pane="topLeft" sqref="G25"/>
+      <selection activeCell="E16" activeCellId="0" pane="topLeft" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1062,40 +1056,45 @@
         <v>89</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
@@ -1103,68 +1102,62 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
+        <v>103</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>107</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="29">
+        <v>108</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
@@ -1172,42 +1165,22 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
-      <c r="A31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="0" t="s">
+      <c r="F30" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="G30" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>